<commit_message>
Add new fakers OZON
</commit_message>
<xml_diff>
--- a/Excel/FakerTickets.xlsx
+++ b/Excel/FakerTickets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BUH\Documents\HatsAndCaps\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF17597-3084-440D-A53F-D9850CCDDCD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B88CF8-2B75-4D53-8776-94D936F36519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11E619BA-09E3-4ADA-8A2B-93B5B1052CD8}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="62">
   <si>
     <t>Фейкер</t>
   </si>
@@ -211,6 +211,18 @@
   </si>
   <si>
     <t>https://www.ozon.ru/seller/disha-167928/</t>
+  </si>
+  <si>
+    <t>ShopShop</t>
+  </si>
+  <si>
+    <t>FoxShop</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/seller/shopshop-126942/</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/seller/foxshop-150482/</t>
   </si>
 </sst>
 </file>
@@ -677,10 +689,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1197BD2E-502D-47A0-A68C-07226AA3551B}">
   <sheetPr codeName="Лист1"/>
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1291,6 +1303,22 @@
       </c>
       <c r="E32" s="4" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1348,8 +1376,10 @@
     <hyperlink ref="E30" r:id="rId26" xr:uid="{F8D2D24D-820F-4E47-9F7D-1F8ADBD79E53}"/>
     <hyperlink ref="E31" r:id="rId27" xr:uid="{87CA6537-60B7-4D49-BA60-46991FF5F8A1}"/>
     <hyperlink ref="E32" r:id="rId28" xr:uid="{EE7E7258-F53D-4229-916A-15318C729345}"/>
+    <hyperlink ref="E33" r:id="rId29" xr:uid="{5D7A0D7C-2063-4285-917C-A7BBB6D6E62B}"/>
+    <hyperlink ref="E34" r:id="rId30" xr:uid="{D5C68FF4-A996-4A82-BE5D-8F71148730E8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ozon fakers status upd
</commit_message>
<xml_diff>
--- a/Excel/FakerTickets.xlsx
+++ b/Excel/FakerTickets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BUH\Documents\HatsAndCaps\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9ED653-D259-41AB-8514-84572CF7515C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D586250-A389-4721-86A2-39FF1FAAFE55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{11E619BA-09E3-4ADA-8A2B-93B5B1052CD8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11E619BA-09E3-4ADA-8A2B-93B5B1052CD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Fakers" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="167">
   <si>
     <t>Фейкер</t>
   </si>
@@ -1827,11 +1827,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1197BD2E-502D-47A0-A68C-07226AA3551B}">
   <sheetPr codeName="Лист1"/>
-  <dimension ref="A1:L59"/>
+  <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E60" sqref="E60"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2991,7 +2991,7 @@
         <v>17616688</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>13</v>
@@ -3008,7 +3008,7 @@
         <v>17616758</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>13</v>
@@ -3025,7 +3025,7 @@
         <v>17616832</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>5</v>
@@ -3042,7 +3042,7 @@
         <v>17618913</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>5</v>
@@ -3059,7 +3059,7 @@
         <v>17619616</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>5</v>
@@ -3076,7 +3076,7 @@
         <v>17619641</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>5</v>
@@ -3093,7 +3093,7 @@
         <v>17628150</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>5</v>
@@ -3110,10 +3110,10 @@
         <v>17782714</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>107</v>
@@ -3127,10 +3127,10 @@
         <v>17782956</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>109</v>
@@ -3144,13 +3144,64 @@
         <v>113</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B60" s="2">
+        <v>17813456</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B61" s="2">
+        <v>17813535</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B62" s="2">
+        <v>17813484</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -3238,9 +3289,10 @@
     <hyperlink ref="E57" r:id="rId53" xr:uid="{947A3EE4-9725-4535-80F9-576BD0540185}"/>
     <hyperlink ref="E58" r:id="rId54" xr:uid="{9FCA9D3B-202E-47DB-8AF2-47FA73A85EDE}"/>
     <hyperlink ref="E59" r:id="rId55" xr:uid="{431E43EB-B206-44F5-AC14-F48FACC2FA35}"/>
+    <hyperlink ref="E60" r:id="rId56" xr:uid="{C0B1282D-DA0B-4D3F-957D-69D065A2040E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId56"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId57"/>
 </worksheet>
 </file>
 
@@ -3461,7 +3513,7 @@
   <sheetPr codeName="Лист3"/>
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -3488,7 +3540,7 @@
         <v>139</v>
       </c>
       <c r="B2" t="str">
-        <f>VLOOKUP(A2,C:C,1,0)</f>
+        <f t="shared" ref="B2:B15" si="0">VLOOKUP(A2,C:C,1,0)</f>
         <v>https://www.ozon.ru/product/beysbolka-588649509</v>
       </c>
       <c r="C2" t="s">
@@ -3500,7 +3552,7 @@
         <v>135</v>
       </c>
       <c r="B3" t="str">
-        <f>VLOOKUP(A3,C:C,1,0)</f>
+        <f t="shared" si="0"/>
         <v>https://www.ozon.ru/product/beysbolka-588663745</v>
       </c>
       <c r="C3" t="s">
@@ -3512,7 +3564,7 @@
         <v>118</v>
       </c>
       <c r="B4" t="str">
-        <f>VLOOKUP(A4,C:C,1,0)</f>
+        <f t="shared" si="0"/>
         <v>https://www.ozon.ru/product/beysbolka-house-time-596044503</v>
       </c>
       <c r="C4" t="s">
@@ -3524,7 +3576,7 @@
         <v>141</v>
       </c>
       <c r="B5" t="str">
-        <f>VLOOKUP(A5,C:C,1,0)</f>
+        <f t="shared" si="0"/>
         <v>https://www.ozon.ru/product/beysbolka-house-time-596045798</v>
       </c>
       <c r="C5" t="s">
@@ -3536,7 +3588,7 @@
         <v>120</v>
       </c>
       <c r="B6" t="str">
-        <f>VLOOKUP(A6,C:C,1,0)</f>
+        <f t="shared" si="0"/>
         <v>https://www.ozon.ru/product/beysbolka-house-time-596048358</v>
       </c>
       <c r="C6" t="s">
@@ -3548,7 +3600,7 @@
         <v>137</v>
       </c>
       <c r="B7" t="str">
-        <f>VLOOKUP(A7,C:C,1,0)</f>
+        <f t="shared" si="0"/>
         <v>https://www.ozon.ru/product/beysbolka-house-time-596049413</v>
       </c>
       <c r="C7" t="s">
@@ -3560,7 +3612,7 @@
         <v>114</v>
       </c>
       <c r="B8" t="str">
-        <f>VLOOKUP(A8,C:C,1,0)</f>
+        <f t="shared" si="0"/>
         <v>https://www.ozon.ru/product/beysbolka-house-time-596050575</v>
       </c>
       <c r="C8" t="s">
@@ -3572,7 +3624,7 @@
         <v>131</v>
       </c>
       <c r="B9" t="str">
-        <f>VLOOKUP(A9,C:C,1,0)</f>
+        <f t="shared" si="0"/>
         <v>https://www.ozon.ru/product/beysbolka-house-time-596050723</v>
       </c>
       <c r="C9" t="s">
@@ -3584,7 +3636,7 @@
         <v>133</v>
       </c>
       <c r="B10" t="str">
-        <f>VLOOKUP(A10,C:C,1,0)</f>
+        <f t="shared" si="0"/>
         <v>https://www.ozon.ru/product/beysbolka-house-time-596535943</v>
       </c>
       <c r="C10" t="s">
@@ -3596,7 +3648,7 @@
         <v>116</v>
       </c>
       <c r="B11" t="e">
-        <f>VLOOKUP(A11,C:C,1,0)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="C11" t="s">
@@ -3608,7 +3660,7 @@
         <v>122</v>
       </c>
       <c r="B12" t="e">
-        <f>VLOOKUP(A12,C:C,1,0)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="C12" t="s">
@@ -3620,7 +3672,7 @@
         <v>124</v>
       </c>
       <c r="B13" t="e">
-        <f>VLOOKUP(A13,C:C,1,0)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="C13" t="s">
@@ -3632,7 +3684,7 @@
         <v>127</v>
       </c>
       <c r="B14" t="e">
-        <f>VLOOKUP(A14,C:C,1,0)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="C14" t="s">
@@ -3644,7 +3696,7 @@
         <v>129</v>
       </c>
       <c r="B15" t="e">
-        <f>VLOOKUP(A15,C:C,1,0)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="C15" t="s">

</xml_diff>

<commit_message>
Ozon fakers new tickets
</commit_message>
<xml_diff>
--- a/Excel/FakerTickets.xlsx
+++ b/Excel/FakerTickets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BUH\Documents\HatsAndCaps\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59909FE-274F-4073-BE09-8EEC74C3BE5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D727CCA8-CEAE-4AC5-9311-1F4D21061797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11E619BA-09E3-4ADA-8A2B-93B5B1052CD8}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Fakers!$A$1:$F$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Лист1!$A$1:$D$77</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Лист1!$A$1:$D$50</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Проверка!$A$1:$C$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="189">
   <si>
     <t>Фейкер</t>
   </si>
@@ -543,82 +543,94 @@
     <t>Loginov-truck</t>
   </si>
   <si>
-    <t>https://www.ozon.ru/product/beysbolka-sb-animal-594686045</t>
-  </si>
-  <si>
-    <t>https://cdn0.ozone.ru/s3/multimedia-d/6329620693.jpg</t>
-  </si>
-  <si>
-    <t>https://www.ozon.ru/product/beysbolka-sb-animal-588996663</t>
-  </si>
-  <si>
-    <t>https://cdn0.ozone.ru/s3/multimedia-7/6325137103.jpg</t>
-  </si>
-  <si>
-    <t>https://www.ozon.ru/product/beysbolka-sb-zhivotnye-584439664</t>
-  </si>
-  <si>
-    <t>https://cdn0.ozone.ru/s3/multimedia-q/6321159734.jpg</t>
-  </si>
-  <si>
-    <t>https://www.ozon.ru/product/beysbolka-sb-animal-594667372</t>
-  </si>
-  <si>
-    <t>https://cdn0.ozone.ru/s3/multimedia-b/6329610215.jpg</t>
-  </si>
-  <si>
-    <t>https://www.ozon.ru/product/beysbolka-sb-animal-588336999</t>
-  </si>
-  <si>
-    <t>https://cdn0.ozone.ru/s3/multimedia-s/6324732880.jpg</t>
-  </si>
-  <si>
-    <t>https://www.ozon.ru/product/beysbolka-sb-zhivotnye-584384525</t>
-  </si>
-  <si>
-    <t>https://cdn0.ozone.ru/s3/multimedia-0/6321161652.jpg</t>
-  </si>
-  <si>
     <t>Myshop</t>
   </si>
   <si>
     <t>https://www.ozon.ru/seller/myshop-465873</t>
   </si>
   <si>
-    <t>https://www.ozon.ru/product/beysbolka-formennaya-goorin-brothers-623143176</t>
-  </si>
-  <si>
-    <t>https://cdn1.ozone.ru/s3/multimedia-2/6355643786.jpg</t>
-  </si>
-  <si>
-    <t>https://www.ozon.ru/product/beysbolka-formennaya-goorin-brothers-623135236</t>
-  </si>
-  <si>
-    <t>https://cdn1.ozone.ru/s3/multimedia-m/6355631998.jpg</t>
-  </si>
-  <si>
-    <t>https://www.ozon.ru/product/beysbolka-tennisnaya-goorin-brothers-623150493</t>
-  </si>
-  <si>
-    <t>https://cdn1.ozone.ru/s3/multimedia-c/6355637208.jpg</t>
-  </si>
-  <si>
-    <t>https://www.ozon.ru/product/beysbolka-tennisnaya-goorin-brothers-623121484</t>
-  </si>
-  <si>
-    <t>https://cdn1.ozone.ru/s3/multimedia-y/6355521670.jpg</t>
-  </si>
-  <si>
-    <t>https://www.ozon.ru/product/beysbolka-formennaya-539670213</t>
-  </si>
-  <si>
-    <t>https://cdn1.ozone.ru/s3/multimedia-k/6283510640.jpg</t>
-  </si>
-  <si>
     <t>Safro</t>
   </si>
   <si>
     <t>https://www.ozon.ru/seller/safro-280653/</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/beysbolka-625338475</t>
+  </si>
+  <si>
+    <t>https://cdn1.ozone.ru/s3/multimedia-2/6356598830.jpg</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/beysbolka-625330064</t>
+  </si>
+  <si>
+    <t>https://cdn1.ozone.ru/s3/multimedia-l/6356586789.jpg</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/beysbolka-625338891</t>
+  </si>
+  <si>
+    <t>https://cdn1.ozone.ru/s3/multimedia-3/6356594943.jpg</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/beysbolka-625383339</t>
+  </si>
+  <si>
+    <t>https://cdn1.ozone.ru/s3/multimedia-b/6356603987.jpg</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/beysbolka-625335012</t>
+  </si>
+  <si>
+    <t>https://cdn1.ozone.ru/s3/multimedia-2/6356588390.jpg</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/beysbolka-625329601</t>
+  </si>
+  <si>
+    <t>https://cdn1.ozone.ru/s3/multimedia-4/6356584432.jpg</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/beysbolka-625337603</t>
+  </si>
+  <si>
+    <t>https://cdn1.ozone.ru/s3/multimedia-q/6356591186.jpg</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/beysbolka-625315566</t>
+  </si>
+  <si>
+    <t>https://cdn1.ozone.ru/s3/multimedia-w/6356573192.jpg</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/beysbolka-625315768</t>
+  </si>
+  <si>
+    <t>https://cdn1.ozone.ru/s3/multimedia-v/6356571103.jpg</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/beysbolka-625339329</t>
+  </si>
+  <si>
+    <t>https://cdn1.ozone.ru/s3/multimedia-r/6356602275.jpg</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/beysbolka-600715311</t>
+  </si>
+  <si>
+    <t>https://cdn1.ozone.ru/s3/multimedia-x/6334950225.jpg</t>
+  </si>
+  <si>
+    <t>ИП Трушникова</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/seller/ip-trushnikova-357628/</t>
+  </si>
+  <si>
+    <t>RocknRolla</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/seller/rocknrolla-139062/</t>
   </si>
 </sst>
 </file>
@@ -876,561 +888,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>149225</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>24342</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1927225</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>2395009</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Рисунок 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AEBFFE3-F359-4EEC-A1FE-BFE0E7ED12A5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="149225" y="214842"/>
-          <a:ext cx="1778000" cy="2370667"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>149225</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>24342</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1927225</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>2395009</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Рисунок 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1690788-ABAC-4E17-9DFD-40EAF4FAF51A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="149225" y="2634192"/>
-          <a:ext cx="1778000" cy="2370667"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>149225</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>24342</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1927225</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>2395009</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Рисунок 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10FB724D-071F-462B-9A0A-27D7510B2CFE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="149225" y="5053542"/>
-          <a:ext cx="1778000" cy="2370667"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>149225</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>24341</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1927225</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>2395008</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Рисунок 15">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8435192-4635-410A-922E-C326DE49F63B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="149225" y="7472891"/>
-          <a:ext cx="1778000" cy="2370667"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>149225</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>21896</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1927225</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>1664028</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="24" name="Рисунок 23">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43E24764-31F2-4BD5-87D4-3CE16E1E7969}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="149225" y="12423446"/>
-          <a:ext cx="1778000" cy="1642132"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>149225</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>24563</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1927225</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>1775661</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="28" name="Рисунок 27">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{262B3E7C-9F61-461D-9ECC-27A9AE7623CE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="149225" y="14112038"/>
-          <a:ext cx="1778000" cy="1751098"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>149225</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>24341</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1927225</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>2395008</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="30" name="Рисунок 29">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDA3CD0E-C381-4A5E-B600-ABB12846348C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="149225" y="15912041"/>
-          <a:ext cx="1778000" cy="2370667"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>149225</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1927225</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>1803400</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="32" name="Рисунок 31">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0895E60B-9EE0-408B-8CB8-4DF4FBB8FEFE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="149225" y="18332450"/>
-          <a:ext cx="1778000" cy="1778000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>149225</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>22786</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1927225</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>1625040</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="34" name="Рисунок 33">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D83FAA02-A20B-43A6-8EB4-C2A1C83B0422}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="149225" y="20158636"/>
-          <a:ext cx="1778000" cy="1602254"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>149225</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1927225</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>1803400</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="38" name="Рисунок 37">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8411E974-10E6-4117-8E1A-F9CF62FFF098}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="149225" y="24228425"/>
-          <a:ext cx="1778000" cy="1778000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>149225</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>22644</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1927225</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>1444208</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="50" name="Рисунок 49">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFFBAD68-BD52-4630-BCC2-A76A0D077E20}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="149225" y="37579719"/>
-          <a:ext cx="1778000" cy="1421564"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1731,11 +1188,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1197BD2E-502D-47A0-A68C-07226AA3551B}">
   <sheetPr codeName="Лист1"/>
-  <dimension ref="A1:L68"/>
+  <dimension ref="A1:L70"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D68" sqref="D68"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3178,7 +2635,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="B67" s="2">
         <v>18091704</v>
@@ -3190,12 +2647,12 @@
         <v>5</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>183</v>
+        <v>161</v>
       </c>
       <c r="B68" s="2">
         <v>18091905</v>
@@ -3207,7 +2664,41 @@
         <v>5</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>184</v>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B69" s="2">
+        <v>18115615</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B70" s="2">
+        <v>18116237</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -3296,19 +2787,20 @@
     <hyperlink ref="E58" r:id="rId54" xr:uid="{9FCA9D3B-202E-47DB-8AF2-47FA73A85EDE}"/>
     <hyperlink ref="E59" r:id="rId55" xr:uid="{431E43EB-B206-44F5-AC14-F48FACC2FA35}"/>
     <hyperlink ref="E60" r:id="rId56" xr:uid="{C0B1282D-DA0B-4D3F-957D-69D065A2040E}"/>
+    <hyperlink ref="E69" r:id="rId57" xr:uid="{CF2A36CC-E195-4A22-B437-84BAE6F83E8F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId57"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId58"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40BD0112-4DA4-46CA-AE15-C6519D5A752D}">
   <sheetPr codeName="Лист2"/>
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2:C12"/>
     </sheetView>
   </sheetViews>
@@ -3334,138 +2826,105 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="190.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="190.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="190.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="190.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="133.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="141.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="190.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="144" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="2">
-        <v>1</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="130.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="2">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="144" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="2">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="115.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="2">
-        <v>1</v>
-      </c>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D75" s="18"/>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="18"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D77" xr:uid="{40BD0112-4DA4-46CA-AE15-C6519D5A752D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D75">
-      <sortCondition descending="1" ref="C1:C77"/>
+  <autoFilter ref="A1:D50" xr:uid="{40BD0112-4DA4-46CA-AE15-C6519D5A752D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D48">
+      <sortCondition descending="1" ref="C1:C50"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D276">
-    <sortCondition ref="B2:B276"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D249">
+    <sortCondition ref="B2:B249"/>
   </sortState>
   <conditionalFormatting sqref="A1:D1048576">
     <cfRule type="expression" dxfId="1" priority="3">
@@ -3477,7 +2936,6 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>